<commit_message>
Implement BOM database features and fix Excel upload mapping
</commit_message>
<xml_diff>
--- a/Weekly_Menu_Categorized.xlsx
+++ b/Weekly_Menu_Categorized.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVSHREE PATIL\OneDrive\Documents\Vs Code\food-management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaun\Desktop\Food Website\Food Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1452DE87-C4AB-46AA-99C1-C37858C668E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D684F711-6EBB-4F85-BD46-EE98D585145B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="125">
   <si>
     <t>Day</t>
   </si>
@@ -322,9 +322,6 @@
     <t>Cabbage Channa Dry</t>
   </si>
   <si>
-    <t>Rajam Masala</t>
-  </si>
-  <si>
     <t>Dal Tadak</t>
   </si>
   <si>
@@ -392,6 +389,12 @@
   </si>
   <si>
     <t>Brunch</t>
+  </si>
+  <si>
+    <t>Item 6</t>
+  </si>
+  <si>
+    <t>Rajama Masala</t>
   </si>
 </sst>
 </file>
@@ -733,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8FC61DF-9F1C-40BC-9E4F-26160833608C}">
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,6 +773,9 @@
       <c r="H1" t="s">
         <v>49</v>
       </c>
+      <c r="I1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -989,7 +995,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1018,7 +1024,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -1047,7 +1053,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -1067,7 +1073,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -1700,10 +1706,10 @@
         <v>99</v>
       </c>
       <c r="E53" t="s">
+        <v>124</v>
+      </c>
+      <c r="F53" t="s">
         <v>100</v>
-      </c>
-      <c r="F53" t="s">
-        <v>101</v>
       </c>
       <c r="G53" t="s">
         <v>87</v>
@@ -1788,13 +1794,13 @@
         <v>5</v>
       </c>
       <c r="D58" t="s">
+        <v>101</v>
+      </c>
+      <c r="E58" t="s">
         <v>102</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>103</v>
-      </c>
-      <c r="F58" t="s">
-        <v>104</v>
       </c>
       <c r="G58" t="s">
         <v>72</v>
@@ -1831,10 +1837,10 @@
         <v>5</v>
       </c>
       <c r="D60" t="s">
+        <v>104</v>
+      </c>
+      <c r="E60" t="s">
         <v>105</v>
-      </c>
-      <c r="E60" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -1893,13 +1899,13 @@
         <v>5</v>
       </c>
       <c r="D64" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" t="s">
         <v>107</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>108</v>
-      </c>
-      <c r="F64" t="s">
-        <v>109</v>
       </c>
       <c r="G64" t="s">
         <v>91</v>
@@ -1984,10 +1990,10 @@
         <v>5</v>
       </c>
       <c r="D69" t="s">
+        <v>109</v>
+      </c>
+      <c r="E69" t="s">
         <v>110</v>
-      </c>
-      <c r="E69" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -2001,7 +2007,7 @@
         <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E70" t="s">
         <v>59</v>
@@ -2021,13 +2027,13 @@
         <v>5</v>
       </c>
       <c r="D71" t="s">
+        <v>112</v>
+      </c>
+      <c r="E71" t="s">
         <v>113</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>114</v>
-      </c>
-      <c r="F71" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -2086,13 +2092,13 @@
         <v>5</v>
       </c>
       <c r="D75" t="s">
+        <v>115</v>
+      </c>
+      <c r="E75" t="s">
         <v>116</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" t="s">
         <v>117</v>
-      </c>
-      <c r="F75" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -2109,7 +2115,7 @@
         <v>57</v>
       </c>
       <c r="E76" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F76" t="s">
         <v>59</v>
@@ -2174,13 +2180,13 @@
         <v>5</v>
       </c>
       <c r="D80" t="s">
+        <v>119</v>
+      </c>
+      <c r="E80" t="s">
         <v>120</v>
       </c>
-      <c r="E80" t="s">
+      <c r="F80" t="s">
         <v>121</v>
-      </c>
-      <c r="F80" t="s">
-        <v>122</v>
       </c>
       <c r="G80" t="s">
         <v>87</v>

</xml_diff>